<commit_message>
TcpApp Server / Client Implementation
</commit_message>
<xml_diff>
--- a/Doc/TcpApp Commands.xlsx
+++ b/Doc/TcpApp Commands.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>TcpApp Protocol</t>
   </si>
@@ -38,18 +38,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Welome Message</t>
-  </si>
-  <si>
     <t>Application Name</t>
   </si>
   <si>
     <t>Application Version</t>
   </si>
   <si>
-    <t>TcpApp Version</t>
-  </si>
-  <si>
     <t>List of Commands</t>
   </si>
   <si>
@@ -74,12 +68,6 @@
     <t>Show Help Screen</t>
   </si>
   <si>
-    <t>TcpAppInit</t>
-  </si>
-  <si>
-    <t>TcpAppVersion?</t>
-  </si>
-  <si>
     <t>MinimizeWindow</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>RAW</t>
   </si>
   <si>
-    <t>What to do if command arrive before Init?</t>
-  </si>
-  <si>
     <t>Case insensitive</t>
   </si>
   <si>
@@ -128,30 +113,6 @@
     <t>var strings = re.Matches(baseString).Cast&lt;Match&gt;().Select(m =&gt; m.Value).ToArray();</t>
   </si>
   <si>
-    <t>Argument:  -Name</t>
-  </si>
-  <si>
-    <t>Optional Argument: [-Name]</t>
-  </si>
-  <si>
-    <t>Optional Argument name with value, value shown as type: [-Name &lt;string&gt;]</t>
-  </si>
-  <si>
-    <t>String array type:</t>
-  </si>
-  <si>
-    <t>Get-Process [-Name] &lt;string[]&gt;</t>
-  </si>
-  <si>
-    <t>Get-Process -Name Explorer, Winlogon, Service</t>
-  </si>
-  <si>
-    <t>Power Shell like Syntax:</t>
-  </si>
-  <si>
-    <t>https://docs.microsoft.com/en-us/powershell/module/microsoft.powershell.core/about/about_command_syntax?view=powershell-6</t>
-  </si>
-  <si>
     <t>ApplicationName?</t>
   </si>
   <si>
@@ -201,13 +162,70 @@
   </si>
   <si>
     <t>Return object list by alias name.</t>
+  </si>
+  <si>
+    <t>Version?</t>
+  </si>
+  <si>
+    <t>TcpApp Server API Version</t>
+  </si>
+  <si>
+    <t>SignIn</t>
+  </si>
+  <si>
+    <t>SignOut</t>
+  </si>
+  <si>
+    <t>ConnectionID*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ConnectionID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LoginString</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Server verify ConnectionID is unique.
+Update when necessary.
+Reconnect, execute SignIn with returned ConnectionID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Optional) Use LoginString to decide if application is allowed to connect?
+Only before init?</t>
+    </r>
+  </si>
+  <si>
+    <t>System Cmd</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,37 +254,30 @@
       <name val="Arial Unicode MS"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -280,29 +291,46 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,280 +609,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E47"/>
+  <dimension ref="B2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="2" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="42.7109375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:6">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="F4" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="120">
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="30">
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="F20" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="30">
-      <c r="B9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>